<commit_message>
changed description file for round2
</commit_message>
<xml_diff>
--- a/stim_folder/stimuli_round2.xlsx
+++ b/stim_folder/stimuli_round2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amsuni-my.sharepoint.com/personal/a_palmann_uva_nl/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amsuni-my.sharepoint.com/personal/a_palmann_uva_nl/Documents/Desktop/pilot_session/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="14_{11B53856-707B-4BD6-B781-ACA8D5757886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9EE9D669-DAD3-472A-9870-44B74A9CAD39}"/>
+  <xr:revisionPtr revIDLastSave="70" documentId="14_{11B53856-707B-4BD6-B781-ACA8D5757886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A486974-C516-46CA-AB92-FFBB507EE3F2}"/>
   <bookViews>
-    <workbookView xWindow="2120" yWindow="300" windowWidth="12890" windowHeight="9780" xr2:uid="{D27A170F-E560-4421-9B21-38197FA838BC}"/>
+    <workbookView xWindow="3780" yWindow="60" windowWidth="15420" windowHeight="9840" xr2:uid="{D27A170F-E560-4421-9B21-38197FA838BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="140">
   <si>
     <t>round</t>
   </si>
@@ -239,39 +239,6 @@
     <t>old_stim_num</t>
   </si>
   <si>
-    <t>Het schilderij toont gefragmenteerde, hoekige vormen in zwart, wit, groen, en enkele rode cirkels tegen een grijze achtergrond. De elementen worden doorkruist door fijne zwarte lijnen, wat een gevoel van beweging of wanorde geeft. Er is een dynamische stroom gecreëerd door de verspreide schikking van vormen.</t>
-  </si>
-  <si>
-    <t>Het schilderij bestaat uit rechthoekige en vierkante vormen in overlappende lagen van gedempte paarse, blauwe en bruine tinten. De vormen hebben zachte, getextureerde randen en de compositie lijkt in balans. De blokken vormen een symmetrisch patroon met subtiele lichte gebieden.</t>
-  </si>
-  <si>
-    <t>Het schilderij toont een abstracte opstelling met kruisende lijnen en onregelmatige vormen. De kleuren zijn fel rood, geel, blauw en zwart, aangebracht in krachtige streken. De achtergrond bevat gelaagde gebieden met lichtere tinten die enigszins doorschijnend lijken. Vormen en lijnen overlappen elkaar en vormen een dicht geheel. De opstelling is ongelijkmatig met verschillende groottes van vormen over het canvas.</t>
-  </si>
-  <si>
-    <t>Het schilderij toont abstracte, gebogen vormen in levendige kleuren zoals groen, oranje, blauw en rood op een zwarte achtergrond. Deze vormen overlappen en verweven, wat een gevoel van energie en beweging geeft. De randen van de vormen zijn licht getextureerd.</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>Het schilderij bestaat uit elkaar kruisende dunne zwarte lijnen die vierkanten en rechthoeken van verschillende groottes vormen. Sommige van deze vormen zijn gevuld met effen kleuren zoals blauw, rood, geel en zwart, terwijl andere leeg blijven. De kleuren zijn asymmetrisch verspreid over het doek, wat zorgt voor een gevoel van balans en ritme. Er is een duidelijk contrast tussen de primaire kleuren en de witte achtergrond.</t>
-  </si>
-  <si>
-    <t>Het schilderij toont een sterk getextureerd oppervlak met aardetinten zoals bruin, grijs en donkergroen. De textuur geeft het een ruwe, bijna steenachtige uitstraling. De donkere kleuren vloeien in elkaar over met subtiele variaties, terwijl lichtere accenten op bepaalde plekken naar voren komen. Er is een abstracte figuur of vorm in het midden, maar de contouren zijn niet duidelijk gedefinieerd.</t>
-  </si>
-  <si>
-    <t>Het schiljderij wordt gekenmerkt door verticale penseelstreken in tinten van roodbruin en beige. De streken zijn ongelijkmatig, waardoor de textuur van het doek eronder zichtbaar wordt. Een zwarte rand omringt het centrale gebied, met enkele onregelmatige, gebogen lijnen die de omlijsting accentueren. Het schilderij heeft een abstracte, gelaagde uitstraling, met subtiele kleurovergangen aan de randen.</t>
-  </si>
-  <si>
-    <t>Het schilderij bestaat uit meerdere ruw getekende rechthoeken die in elkaar overlopen. De achtergrond en de rechthoeken hebben een neutraal beige kleurenpalet. Er is weinig contrast en de lijnen zijn schetsmatig en ongelijk, wat een informele en subtiele textuur geeft.</t>
-  </si>
-  <si>
-    <t>Het schilderij toont een dynamische compositie met gelaagde vormen en kleuren. Overheersende tonen zijn wit, rood en beige, met verspreide lineaire elementen en kleurvlakken. De opstelling is chaotisch, met overlappende texturen en gedurfde, expressieve penseelstreken.</t>
-  </si>
-  <si>
-    <t>Het schilderij bestaat uit onregelmatige rechthoekige en vierkante vormen in een patchwork-compositie. De kleuren variëren van zachte geel- en bruintinten tot gedempte groenen, roodtinten en oranje. Enkele delen bevatten strepen van wisselende breedte, wat een ritmisch element toevoegt. De penseelstreken zijn zacht, met een aquarelachtige textuur. Over het geheel voelt het werk evenwichtig maar asymmetrisch aan.</t>
-  </si>
-  <si>
     <t>img_16</t>
   </si>
   <si>
@@ -320,9 +287,6 @@
     <t>m_Motherwell-AP-26.tif</t>
   </si>
   <si>
-    <t>Het schilderij toont een dynamische compositie van draaiende, donkere vormen afgewisseld met levendige kleuren zoals rood, blauw, geel en groen. Een sterke diagonale witte lijn snijdt door het beeld en creëert een gevoel van scheiding en beweging. De texturen zijn vloeiend en organisch, alsof het vloeibare patronen of geabstraheerde landschappen zijn. Het spel van licht en donker roept diepte op.</t>
-  </si>
-  <si>
     <t>Louis-AP-07.tif</t>
   </si>
   <si>
@@ -338,9 +302,6 @@
     <t>Motherwell 94 Night Music Opus No. 7.tif</t>
   </si>
   <si>
-    <t>Het schilderij toont een vereenvoudigde, symmetrische vorm in gedempte tinten bruin, rood en zwart. De kleuren zijn zacht gemengd, zonder scherpe randen, wat een gevoel van rust en gewicht creëert. De compositie suggereert een monumentale, sculpturale aanwezigheid.</t>
-  </si>
-  <si>
     <t>m_Francis-AP-20.tif</t>
   </si>
   <si>
@@ -374,9 +335,6 @@
     <t>m_Frankenthaler 143 Madame de Pomoadour.tif</t>
   </si>
   <si>
-    <t>Het schilderij bestaat uit dunne, gebogen en elkaar kruisende lijnen in lichtbruine en zwarte tinten op een beige achtergrond. Er zijn vervaagde bruine vlekken die in de achtergrond opgaan. De lijnen zijn abstract en lijken geen duidelijke geometrische structuur te hebben. In de linkerbovenhoek is een vage markering te zien die lijkt op handschrift.</t>
-  </si>
-  <si>
     <t>Moholy-Nagy 24 Am 4(26).tif</t>
   </si>
   <si>
@@ -389,9 +347,6 @@
     <t>2 Malewitsch - Suprematismus.. Malerischer Realismus eines Fussballspielers.tif</t>
   </si>
   <si>
-    <t>Het schilderij toont geometrische vormen met scherpe hoeken, zoals rechthoeken en driehoeken, op een zwarte en lichtgekleurde achtergrond. Centraal staan twee bollen met zachte schaduwen, waarvan één groter is dan de andere. De achtergrond bevat delen in wit, groen en lichtgrijs. De compositie benadrukt een balans tussen lichte en donkere gebieden.</t>
-  </si>
-  <si>
     <t>img_36</t>
   </si>
   <si>
@@ -425,9 +380,6 @@
     <t>Smith-PA-29.tif</t>
   </si>
   <si>
-    <t>Het schilderij toont een raster van kleine, kleurrijke vierkanten die in een mozaïekachtig patroon zijn gerangschikt. De kleuren variëren, waaronder tinten blauw, rood, geel, groen en zwart, wat een levendig, gepixeld effect creëert. De ordening is onregelmatig, met kleuren die subtiele overgangen vormen en zonder een duidelijk middelpunt. Het geeft de indruk van een abstract, textuurachtig oppervlak.</t>
-  </si>
-  <si>
     <t>img_40</t>
   </si>
   <si>
@@ -443,35 +395,137 @@
     <t>Rothko-RR-05.tif</t>
   </si>
   <si>
-    <t>Het schilderij toont een symmetrische opstelling van witte en grijze rechthoekige vormen, verticaal gestapeld op een zwarte achtergrond. De rechthoeken worden smaller naarmate ze naar het midden bewegen, wat een uitgebalanceerde, geometrische structuur creëert. De vormen hebben een licht getextureerd oppervlak en de zwarte achtergrond is egaal. De compositie voelt precies en gestructureerd aan.</t>
-  </si>
-  <si>
     <t>AI_desc_img</t>
   </si>
   <si>
     <t>stim_num</t>
   </si>
   <si>
-    <t>Het schilderij bevat abstracte vormen met overwegend rode en witte tinten, vermengd met zachte blauwe en groene accenten. Brede, vloeiende penseelstreken overlappen elkaar in een gelaagde compositie. Sommige rode gebieden lijken op langgerekte figuren of gebaren, maar de vormen blijven vaag.</t>
-  </si>
-  <si>
-    <t>round2</t>
-  </si>
-  <si>
-    <t>round3</t>
-  </si>
-  <si>
-    <t>Het schilderij toont een dynamische compositie van abstracte vormen in donkerblauw, geel en rood. De achtergrond is lichtbeige. De vormen lijken gefragmenteerd en verspreid over het doek, met spetters en druppels verf die beweging suggereren. Dunne zwarte lijnen zijn zichtbaar en kruisen of omlijnen sommige vormen. De verf lijkt in lagen aangebracht, met sommige delen dikker en textuurvoller dan andere.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Het schilderij toont een getextureerde achtergrond met voornamelijk blauwe en roze tinten. Een centrale, onregelmatige ovale vorm met ruwe, abstracte markeringen is roze met oranje en rode accenten. Verschillende geometrische vormen zijn erbovenop geplaatst, waaronder zwarte, gele, blauwe en groene elementen. Sommige vormen zijn langwerpig en scherp, terwijl andere rond of onregelmatig zijn. </t>
+    <t>Het schilderij toont gefragmenteerde, hoekige vormen in zwart, wit en groen tegen een grijze achtergrond. De elementen worden doorkruist door fijne zwarte lijnen, wat een gevoel van beweging geeft. Er zit dynamiek in door de verspreiding van de vormen over het schilderij.</t>
+  </si>
+  <si>
+    <t>Het schilderij bestaat uit rechthoekige en vierkante vormen in overlappende lagen van gedempte paarse, blauwe en bruine tinten. De vormen hebben zachte, getextureerde randen en de compositie lijkt in balans te zijn. De blokken vormen een gelaagd patroon met subtiele lichte gebieden.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Het schilderij toont een ongelijkmatige opstelling met kruisende vormen van verschillende groottes en zonder duidelijke omlijning. De kleuren zijn fel rood, geel en blauw, aangebracht in krachtige streken. De achtergrond bevat lagen van verschillende tinten die ietwat doorschijnend zijn. </t>
+  </si>
+  <si>
+    <t>In het midden van het schilderij staat een onregelmatige, ovale vorm. Deze is ruw en abstract en daarbovenop zijn verschillende geometrische en organische vormen geplaatst. De vormen verschillen in grootte en richting, waardoor het geheel beweeglijk lijkt. Sommige zijn lang en scherp, andere hebben een ronde vorm.</t>
+  </si>
+  <si>
+    <t>Het schilderij toont abstracte figuren in levendige kleuren zoals groen, oranje, blauw en rood op een donkere achtergrond. De vormen overlappen en zijn verweven met elkaar. De randen van de vormen zijn zacht.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Het schilderij toont een raster van kleine, kleurrijke vierkanten die in een mozaïekachtig patroon zijn gerangschikt. De kleuren variëren, waaronder tinten blauw, rood, geel, groen en zwart. De ordening is onregelmatig, met kleuren die subtiele overgangen vormen en zonder een duidelijk middelpunt. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Het schilderij toont een simpele, symmetrische vorm in gedempte tinten bruin, rood en zwart. De kleuren zijn zacht gemengd, zonder scherpe randen, wat een gevoel van rust en gewicht creëert. </t>
+  </si>
+  <si>
+    <t>Het schilderij bevat abstracte vormen met rode en witte tinten, vermengd met licht blauwe en groene accenten. Brede, vloeiende penseelstreken overlappen elkaar in een gelaagde compositie. Sommige gebieden lijken op langgerekte figuren of gebaren, maar de vormen blijven vaag.</t>
+  </si>
+  <si>
+    <t>Het schilderij bestaat uit elkaar kruisende dunne zwarte lijnsegmenten die verschillende vormen creëren. Sommige van deze vormen zijn gevuld met effen kleuren zoals blauw, rood, geel en zwart, terwijl andere leeg blijven. De kleuren zijn asymmetrisch verspreid over het doek.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Het schilderij toont een sterk getextureerd oppervlak met aardetinten zoals bruin, grijs en donkergroen. De textuur geeft het een ruwe, bijna steenachtige uitstraling. De donkere kleuren vloeien in elkaar over met subtiele variaties, terwijl lichtere accenten op bepaalde plekken naar voren komen. </t>
+  </si>
+  <si>
+    <t>Het schilderij wordt gekenmerkt door verticale, ongelijkmatige penseelstreken in tinten van rood en roze. Een zwarte rand omringt het centrale gebied, met enkele onregelmatige, gebogen lijnen die de omlijsting accentueren. Het schilderij heeft een abstracte, gelaagde uitstraling, met subtiele kleurovergangen aan de randen.</t>
+  </si>
+  <si>
+    <t>Het schilderij bestaat uit meerdere losjes getekende rechthoeken die in elkaar overlopen. De achtergrond en de rechthoeken hebben een neutraal beige kleurenpalet. Er is weinig contrast en de lijnen zijn schetsmatig en ongelijk.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Het schilderij toont een dynamische compositie </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>en creëert de illusie van driedimensionale balken en vormen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Overheersende tonen zijn wit, rood en beige, met verspreide lineaire elementen en kleurvlakken.  De opstelling is chaotisch, met overlappende texturen en expressieve penseelstreken en er is een rood vierkant aan de rechterbovenkant.</t>
+    </r>
+  </si>
+  <si>
+    <t>Het schilderij toont een symmetrische opstelling van verticaal gestapelde rechthoekige vormen, wat een uitgebalanceerde, geometrische structuur creëert. De vormen hebben een licht getextureerd oppervlak en de achtergrond is egaal. De compositie voelt gestructureerd aan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Het schilderij toont een dynamische compositie van abstracte vormen in donkerblauw, geel en rood. De achtergrond is lichtbeige, wat een contrast vormt met de donkere vormen. Er zijn kleurvlekken die willekeurig lijken, maar toch is eenevenwicht in de compositie behouden, met een lichte onbalans naar rechts. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Het schilderij toont geometrische vormen met scherpe hoeken, zoals rechthoeken en driehoeken, op een zwarte, groene en lichtgrijze achtergrond. Centraal staan twee bollen met zachte schaduwen, waarvan één groter is dan de andere. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>De grotere bol is in de rechter onderhoek geplaatst.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Het schilderij toont een dynamische compositie van draaiende, donkere vormen afgewisseld met levendige kleuren zoals rood, blauw, geel en groen. Een sterke diagonale witte lijn snijdt </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">rechtsboven </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>door het beeld. De texturen zijn vloeiend en organisch. Het spel van licht en donker roept diepte op.</t>
+    </r>
+  </si>
+  <si>
+    <t>Het schilderij bestaat uit onregelmatige vormen in een patchwork-compositie. De kleuren variëren van zachte geel- en bruintinten tot gedempte groenen, roodtinten en oranje. De penseelstreken zijn zacht, met een aquarelachtige textuur. Over het geheel voelt het werk evenwichtig maar asymmetrisch aan.</t>
+  </si>
+  <si>
+    <t>Het schilderij bestaat uit dunne, gebogen en elkaar kruisende lijnen in lichtbruine en zwarte tinten op een beige achtergrond. Er zijn vervaagde bruine vlekken die in de achtergrond opgaan. De lijnen zijn abstract en lijken geen duidelijke geometrische structuur te hebben. In de linkerbovenhoek is een vage markering te zien die lijkt op handtekening.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,27 +547,36 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -549,19 +612,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,10 +647,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -620,7 +692,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -726,7 +798,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -868,7 +940,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -876,17 +948,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03745583-B80B-4024-A0D6-717F369FF5CD}">
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -910,7 +982,7 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="J1" t="s">
         <v>65</v>
@@ -918,11 +990,8 @@
       <c r="K1" t="s">
         <v>66</v>
       </c>
-      <c r="L1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1</v>
       </c>
@@ -950,20 +1019,14 @@
       <c r="I2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>67</v>
+      <c r="J2" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="K2">
         <v>24</v>
       </c>
-      <c r="Q2" t="s">
-        <v>139</v>
-      </c>
-      <c r="R2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>2</v>
       </c>
@@ -991,26 +1054,14 @@
       <c r="I3" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>68</v>
+      <c r="J3" s="6" t="s">
+        <v>122</v>
       </c>
       <c r="K3">
         <v>25</v>
       </c>
-      <c r="O3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P3">
-        <v>14</v>
-      </c>
-      <c r="Q3">
-        <v>7</v>
-      </c>
-      <c r="R3">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1038,26 +1089,14 @@
       <c r="I4" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>69</v>
+      <c r="J4" s="6" t="s">
+        <v>123</v>
       </c>
       <c r="K4">
         <v>3</v>
       </c>
-      <c r="O4" t="s">
-        <v>40</v>
-      </c>
-      <c r="P4">
-        <v>13</v>
-      </c>
-      <c r="Q4">
-        <v>6</v>
-      </c>
-      <c r="R4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1085,26 +1124,14 @@
       <c r="I5" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>142</v>
+      <c r="J5" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="K5">
         <v>4</v>
       </c>
-      <c r="O5" t="s">
-        <v>31</v>
-      </c>
-      <c r="P5">
-        <v>15</v>
-      </c>
-      <c r="Q5">
-        <v>8</v>
-      </c>
-      <c r="R5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1132,20 +1159,14 @@
       <c r="I6" t="s">
         <v>16</v>
       </c>
-      <c r="J6" s="4" t="s">
-        <v>70</v>
+      <c r="J6" s="6" t="s">
+        <v>125</v>
       </c>
       <c r="K6">
         <v>23</v>
       </c>
-      <c r="Q6">
-        <v>21</v>
-      </c>
-      <c r="R6">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1155,32 +1176,32 @@
       <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H7" s="6" t="s">
+      <c r="D7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>40</v>
       </c>
       <c r="I7" t="s">
-        <v>106</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>112</v>
+        <v>93</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>139</v>
       </c>
       <c r="K7">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1190,32 +1211,32 @@
       <c r="C8">
         <v>7</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" t="s">
+        <v>104</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I8" t="s">
-        <v>119</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="K8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1225,32 +1246,32 @@
       <c r="C9">
         <v>8</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="H9" s="6" t="s">
+      <c r="D9" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>31</v>
       </c>
       <c r="I9" t="s">
-        <v>96</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>100</v>
+        <v>84</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>127</v>
       </c>
       <c r="K9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1278,14 +1299,14 @@
       <c r="I10" t="s">
         <v>17</v>
       </c>
-      <c r="J10" s="4" t="s">
-        <v>138</v>
+      <c r="J10" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="K10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1313,14 +1334,14 @@
       <c r="I11" t="s">
         <v>18</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>72</v>
+      <c r="J11" s="6" t="s">
+        <v>129</v>
       </c>
       <c r="K11">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1348,14 +1369,14 @@
       <c r="I12" t="s">
         <v>19</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>73</v>
+      <c r="J12" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="K12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1383,14 +1404,14 @@
       <c r="I13" t="s">
         <v>20</v>
       </c>
-      <c r="J13" s="4" t="s">
-        <v>74</v>
+      <c r="J13" s="6" t="s">
+        <v>131</v>
       </c>
       <c r="K13">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1418,14 +1439,14 @@
       <c r="I14" t="s">
         <v>21</v>
       </c>
-      <c r="J14" t="s">
-        <v>75</v>
+      <c r="J14" s="7" t="s">
+        <v>132</v>
       </c>
       <c r="K14">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:11" ht="16">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1453,14 +1474,14 @@
       <c r="I15" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="5" t="s">
-        <v>76</v>
+      <c r="J15" s="7" t="s">
+        <v>133</v>
       </c>
       <c r="K15">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1470,26 +1491,26 @@
       <c r="C16">
         <v>15</v>
       </c>
-      <c r="D16" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="G16" s="6" t="s">
+      <c r="D16" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" t="s">
+        <v>114</v>
+      </c>
+      <c r="J16" s="6" t="s">
         <v>134</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I16" t="s">
-        <v>130</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>135</v>
       </c>
       <c r="K16">
         <v>7</v>
@@ -1505,26 +1526,26 @@
       <c r="C17">
         <v>16</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="H17" s="6" t="s">
+      <c r="D17" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>40</v>
       </c>
       <c r="I17" t="s">
-        <v>105</v>
-      </c>
-      <c r="J17" t="s">
-        <v>141</v>
+        <v>92</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>135</v>
       </c>
       <c r="K17">
         <v>30</v>
@@ -1540,32 +1561,32 @@
       <c r="C18">
         <v>17</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="H18" s="6" t="s">
+      <c r="D18" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>40</v>
       </c>
       <c r="I18" t="s">
-        <v>118</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>124</v>
+        <v>103</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>109</v>
       </c>
       <c r="K18">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" ht="16">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1575,26 +1596,26 @@
       <c r="C19">
         <v>18</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="G19" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="H19" s="6" t="s">
+      <c r="D19" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I19" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="J19" s="3" t="s">
-        <v>117</v>
+      <c r="I19" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>136</v>
       </c>
       <c r="K19">
         <v>40</v>
@@ -1610,32 +1631,32 @@
       <c r="C20">
         <v>19</v>
       </c>
-      <c r="D20" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>88</v>
+      <c r="D20" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="H20" t="s">
         <v>31</v>
       </c>
       <c r="I20" t="s">
-        <v>79</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>89</v>
+        <v>68</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>78</v>
       </c>
       <c r="K20">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" ht="16">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1645,26 +1666,26 @@
       <c r="C21">
         <v>20</v>
       </c>
-      <c r="D21" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>92</v>
+      <c r="D21" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="H21" t="s">
         <v>40</v>
       </c>
       <c r="I21" t="s">
-        <v>85</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>94</v>
+        <v>74</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="K21">
         <v>31</v>
@@ -1680,26 +1701,26 @@
       <c r="C22">
         <v>21</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>83</v>
+      <c r="D22" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="H22" t="s">
         <v>11</v>
       </c>
       <c r="I22" t="s">
-        <v>78</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="K22">
         <v>26</v>

</xml_diff>